<commit_message>
scrape page from 6 to 10
</commit_message>
<xml_diff>
--- a/mobile_data01.xlsx
+++ b/mobile_data01.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,84 +478,84 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Xiaomi</t>
+          <t>Huawei</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>৳140,000.00</t>
+          <t>Coming soon</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024, February 22</t>
+          <t>2024, April 06</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Android 14, HyperOS</t>
+          <t>EMUI 14, no Google Play Services</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>6.73" 1440x3200 pixels</t>
+          <t>6.67" 1080x2400 pixels</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>50MP 4320p</t>
+          <t>108MP 1080p</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>12/16GB RAM Snapdragon 8 Gen 3</t>
+          <t>8GB RAM Snapdragon 680 4G</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>5000mAh 90W80W</t>
+          <t>4500mAh 66W</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Vivo</t>
+          <t>Huawei</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>৳28,000.00</t>
+          <t>৳60,000.00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024, February 22</t>
+          <t>2024, April 13</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Android 14, Funtouch 14</t>
+          <t>EMUI 14, no Google Play Services</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>6.67" 1080x2400 pixels</t>
+          <t>6.7" 1084x2412 pixels</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>50MP 1080p</t>
+          <t>50MP 2160p</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>6/8GB RAM Snapdragon 4 Gen 2</t>
+          <t>8GB RAM Snapdragon 778G 4G</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>5000mAh 44W</t>
+          <t>4500mAh 66W</t>
         </is>
       </c>
     </row>
@@ -567,380 +567,380 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>৳18,000.00</t>
+          <t>৳35,000.00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024, February 22</t>
+          <t>2024, April 16</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>HarmonyOS 4.0</t>
+          <t>EMUI 14, no Google Play Services</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>6.75" 720x1600 pixels</t>
+          <t>6.7" 1080x2388 pixels</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>13MP 1080p</t>
+          <t>108MP 1080p</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Kirin 710A</t>
+          <t>8GB RAM Snapdragon 680 4G</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>6000mAh Li-Po</t>
+          <t>5000mAh 40W</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Xiaomi</t>
+          <t>Realme</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>৳55,000.00</t>
+          <t>৳33,500.00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024, February 22</t>
+          <t>2024, March 19</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Android 14, HyperOS</t>
+          <t>Android 14, Realme UI 5.0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>12.4" 2032x3048 pixels</t>
+          <t>6.67" 1080x2400 pixels</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>50MP 2160p</t>
+          <t>50MP 1080p</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>8-16GB RAM Snapdragon 8 Gen 2</t>
+          <t>8GB RAM Dimensity 7050</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>10000mAh 120W</t>
+          <t>5000mAh 67W</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Vivo</t>
+          <t>Honor</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>৳60,000.00</t>
+          <t>৳160,000.00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2024, February 22</t>
+          <t>2024, March 22</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Android 14, Funtouch 14</t>
+          <t>Android 14, MagicOS 8</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6.78" 1260x2800 pixels</t>
+          <t>6.8" 1280x2800 pixels</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>50MP 4320p</t>
+          <t>180MP 2160p</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>8/12GB RAM Snapdragon 8 Gen 2</t>
+          <t>24GB RAM Snapdragon 8 Gen 3</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>5160mAh</t>
+          <t>5600mAh 80W66W</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Realme</t>
+          <t>Honor</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>৳40,000.00</t>
+          <t>৳110,000.00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2024, April 22</t>
+          <t>2024, March 22</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Android 14, Realme UI</t>
+          <t>Android 14, MagicOS 8</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6.72" 1080x2400 pixels</t>
+          <t>6.8" 1280x2800 pixels</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>108MP 1080p</t>
+          <t>180MP 2160p</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>6/8GB RAM Snapdragon 685</t>
+          <t>16GB RAM Snapdragon 8 Gen 3</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>5000mAh 33W</t>
+          <t>5600mAh 80W66W</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Lava</t>
+          <t>Infinix</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Coming soon</t>
+          <t>৳38,000.00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Not announced yet</t>
+          <t>2024, March 19</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Android 13</t>
+          <t>Android 14, XOS 14</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>6.5" 720x1600 pixels</t>
+          <t>6.78" 1080x2436 pixels</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>50MP 1080p</t>
+          <t>108MP 1440p</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>8GB RAM Unisoc Tiger T616</t>
+          <t>12GB RAM Dimensity 7020</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>5000mAh Li-Po</t>
+          <t>4600mAh 100W20W</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Oppo</t>
+          <t>Infinix</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Coming soon</t>
+          <t>৳30,999.00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Not announced yet</t>
+          <t>2024, March 19</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Android 14</t>
+          <t>Android 14, XOS 14</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>6.82" 1440x3168 pixels</t>
+          <t>6.78" 1080x2436 pixels</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>50MP 2160p</t>
+          <t>108MP 1440p</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>12/16GB RAM Snapdragon 8 Gen 3</t>
+          <t>8/12GB RAM Helio G99 Ultimate</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>5000mAh Li-Po</t>
+          <t>5000mAh 70W 20W</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Oppo</t>
+          <t>Infinix</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Coming soon</t>
+          <t>৳35,000.00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Not announced yet</t>
+          <t>2024, March 19</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Android 13</t>
+          <t>Android 14, XOS 14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>6.82" 1440x3168 pixels</t>
+          <t>6.78" 1080x2436 pixels</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>50MP 2160p</t>
+          <t>108MP 1440p</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>12/16GB RAM Snapdragon 8 Gen 2</t>
+          <t>8GB RAM Dimensity 7020</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>5000mAh Li-Po</t>
+          <t>5000mAh 45W20W</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Oppo</t>
+          <t>Infinix</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Coming soon</t>
+          <t>৳26,999.00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Not announced yet</t>
+          <t>2024, March 19</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Android 14</t>
+          <t>Android 14, XOS 14</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>6.78" 1264x2780 pixels</t>
+          <t>6.78" 1080x2436 pixels</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>64MP 2160p</t>
+          <t>108MP 1440p</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>12/16GB RAM Dimensity 9300</t>
+          <t>8GB RAM Helio G99 Ultimate</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>5000mAh</t>
+          <t>5000mAh 45W20W</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Xiaomi</t>
+          <t>Symphony</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>৳12,499.00 ৳10,999.00</t>
+          <t>৳11,699.00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2024, February 23</t>
+          <t>2024, March 18</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Android 14, MIUI</t>
+          <t>Android 13</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6.71" 720x1650 pixels</t>
+          <t>6.56" 720x1600 pixels</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>8MP 1080p</t>
+          <t>108MP 1080p</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>3-6GB RAM Helio G36</t>
+          <t>6/8GB RAM UniSOC T616</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>5000mAh 10W</t>
+          <t>5000mAh Li-Po</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>OnePlus</t>
+          <t>Motorola</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -955,22 +955,22 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Android 13</t>
+          <t>Android 14</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>6.72" 1080x2400 pixels</t>
+          <t>6.5" 1080x2400 pixels</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>108MP 1080p</t>
+          <t>50MP 2160p</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>8GB RAM Snapdragon 695 5G</t>
+          <t>4GB RAM Snapdragon 480+ 5G</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -982,7 +982,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>OnePlus</t>
+          <t>Meizu</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -997,44 +997,44 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Android 13</t>
+          <t>Android 14</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>6.7" 1080x2400 pixels</t>
+          <t>6.55" 1080x2340 pixels</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>50MP 2160p</t>
+          <t>200MP 4320p</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>8/12GB RAM Snapdragon 782G</t>
+          <t>8/12GB RAM Snapdragon 8 Gen 3</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>5000mAh Li-Po</t>
+          <t>4800mAh</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>OnePlus</t>
+          <t>Walton</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Coming soon</t>
+          <t>৳13,999.00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Not announced yet</t>
+          <t>2024, March 15</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1044,81 +1044,81 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>6.7" 1080x2400 pixels</t>
+          <t>6.8" 720 x 1612 pixels</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>64MP 2160p</t>
+          <t>52MP 1080P</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>12GB RAM Snapdragon 695 5G</t>
+          <t>8GB RAM UNISOC TIGER T606</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>5000mAh Li-Po</t>
+          <t>6000mAh Li-po</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Huawei</t>
+          <t>Ulefone</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>৳120,000.00</t>
+          <t>৳30,000.00</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Exp. release 2024, March</t>
+          <t>2024, March 14</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>HarmonyOS 4.0</t>
+          <t>Android 13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>6.94" 1136x2690 pixels</t>
+          <t>5.93" 720x1440 pixels</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>50MP 2160p</t>
+          <t>50MP 1080p</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>12/16GB RAM</t>
+          <t>8GB RAM Unisoc Tiger T616</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>4520mAh 66W40W</t>
+          <t>9600mAh 18W</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Oppo</t>
+          <t>Asus</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Coming soon</t>
+          <t>৳110,000.00</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Not announced yet</t>
+          <t>2024, April 14</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1128,39 +1128,39 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>6.7" 1080x2412 pixels</t>
+          <t>6.78" 1080x2400 pixels</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>50MP 2160p</t>
+          <t>50MP 4320p</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>12GB RAM Dimensity 8200</t>
+          <t>12/16GB RAM Snapdragon 8 Gen 3</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>4600mAh Li-Po</t>
+          <t>5500mAh 65W15W</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Oppo</t>
+          <t>Xiaomi</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Coming soon</t>
+          <t>৳23,000.00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Not announced yet</t>
+          <t>2024, March 13</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1170,165 +1170,165 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>6.7" 1080x2412 pixels</t>
+          <t>6.67" 1080x2400 pixels</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>50MP 2160p</t>
+          <t>108MP 1080p</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>8/12GB RAM Dimensity 7050</t>
+          <t>8/12GB RAM Dimensity 6080</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>5000mAh Li-Po</t>
+          <t>5000mAh 33W</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Walton</t>
+          <t>Vivo</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>৳11,999.00</t>
+          <t>৳12,000.00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2024, February 17</t>
+          <t>2024, March 13</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Android 13</t>
+          <t>Android 14, Funtouch 14</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>6.8" 720 x 1612 pixels</t>
+          <t>6.56" 720x1612 pixels</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>52MP 1080P</t>
+          <t>13MP 1080p</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>8GB RAM UNISOC TIGER T606</t>
+          <t>4GB RAM Helio G85</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>5010mAh Li-po</t>
+          <t>5000mAh 15W</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>Realme</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Coming soon</t>
+          <t>৳25,000.00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2023, June 27</t>
+          <t>2024, April 07</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Android 13</t>
+          <t>Android 14, Realme UI 5.0</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>7.6" 1840x2208 pixels</t>
+          <t>6.67" 1080x2400 pixels</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>48MP 2160p</t>
+          <t>50MP 1080p</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>12GB RAM Google Tensor G2</t>
+          <t>12GB RAM Dimensity 6100+</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>4821mAh Li-Po</t>
+          <t>5000mAh 15W</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Oppo</t>
+          <t>Motorola</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>৳30,000.00</t>
+          <t>৳35,000.00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2024, February 08</t>
+          <t>2024, March 22</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Android 14, ColorOS 14</t>
+          <t>Android 14</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6.7" 1080x2412 pixels</t>
+          <t>6.7" 1080x2400 pixels</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>64MP 2160p</t>
+          <t>50MP 1080p</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>8GB RAM Dimensity 7050</t>
+          <t>8GB RAM Dimensity 7020</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>5000mAh Li-Po</t>
+          <t>5000mAh 30W15W</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Energizer</t>
+          <t>Motorola</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Coming soon</t>
+          <t>৳22,000.00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Not announced yet</t>
+          <t>2024, March 21</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1338,133 +1338,133 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>6.78" 1080x2460 pixels</t>
+          <t>6.6" 720x1612 pixels</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>60MP 2160p</t>
+          <t>50MP 1080p</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>4GB RAM Snapdragon 4 Gen 1</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>28000mAh</t>
+          <t>5000mAh 18W</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TCL</t>
+          <t>Vivo</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Coming soon</t>
+          <t>৳29,000.00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Exp. release 2024, March</t>
+          <t>2024, March 13</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Android 14</t>
+          <t>Android 14, Funtouch 14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>6.75" 720x1600 pixels</t>
+          <t>6.67" 1080x2400 pixels</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>50MP 1080p</t>
+          <t>50MP 2160p</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>4GB RAM Helio G35</t>
+          <t>8GB RAM Dimensity 7200</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>5010mAh</t>
+          <t>5000mAh 44W</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Vivo</t>
+          <t>Sony</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>৳55,000.00</t>
+          <t>Coming soon</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2024, March 07</t>
+          <t>Not announced yet</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Android 14, Funtouch 14</t>
+          <t>Android 14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>6.78" 1260x2800 pixels</t>
+          <t>6.1" 1080x2520 pixels</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>50MP 2160p</t>
+          <t>48MP 1080p</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>8/12GB RAM Dimensity 8200</t>
+          <t>6/8GB RAM Snapdragon 695 5G</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>5000mAh 80W</t>
+          <t>5000mAh Li-Po</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Vivo</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>৳59,999.00</t>
+          <t>৳36,000.00</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2024, March 04</t>
+          <t>2024, March 15</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Android 14, Funtouch 14</t>
+          <t>Android 14, One UI 6.1</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>6.78" 1260x2800 pixels</t>
+          <t>6.6" 1080x2340 pixels</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1474,103 +1474,103 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>8/12GB RAM Snapdragon 7 Gen 3</t>
+          <t>6/8/12GB RAM Exynos 1380</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>5000mAh 80W</t>
+          <t>5000mAh 25W</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Vivo</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Coming soon</t>
+          <t>৳43,000.00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Not announced yet</t>
+          <t>2024, March 15</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Android 13</t>
+          <t>Android 14, One UI 6.1</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>6.78" 1080x2400 pixels</t>
+          <t>6.6" 1080x2340 pixels</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>64MP 2160p</t>
+          <t>50MP 2160p</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>8GB RAM Dimensity 7200</t>
+          <t>8/12GB RAM Exynos 1480</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>4600mAh Li-Po</t>
+          <t>5000mAh 25W</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Ulefone</t>
+          <t>Motorola</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>৳40,000.00</t>
+          <t>Coming soon</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2024, January</t>
+          <t>Not announced yet</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Android 13</t>
+          <t>Android 14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>6.78" 1080x2400 pixels</t>
+          <t>6.55" 1080x2400 pixels</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>108MP 1440p</t>
+          <t>50MP 2160p</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>12GB RAM Helio G99</t>
+          <t>8GB RAM Dimensity 8020</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>5050mAh Li-Po</t>
+          <t>4400mAh Li-Po</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Xiaomi</t>
+          <t>Motorola</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1590,7 +1590,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>6.73" 1440x3200 pixels</t>
+          <t>6.67" 1080x2400 pixels</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>12/16GB RAM Snapdragon 8 Gen 2</t>
+          <t>8-18GB RAM Snapdragon 8 Gen 2</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1612,7 +1612,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Realme</t>
+          <t>Motorola</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1632,29 +1632,29 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>6.7" 1080x2412 pixels</t>
+          <t>6.67" 1080x2400 pixels</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>64MP 2160p</t>
+          <t>50MP 4320p</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>8/12GB RAM Snapdragon 7s Gen 2</t>
+          <t>8GB RAM Snapdragon 8 Gen 2</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>5000mAh Li-Po</t>
+          <t>5100mAh Li-Po</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Realme</t>
+          <t>Oppo</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1679,12 +1679,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>50MP 2160p</t>
+          <t>64MP 2160p</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>8GB RAM Snapdragon 6 Gen 1</t>
+          <t>8GB RAM Dimensity 7050</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1696,7 +1696,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Realme</t>
+          <t>ZTE</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1716,29 +1716,29 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>6.43" 1080x2400 pixels</t>
+          <t>6.92" 1080x2460 pixels</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>64MP 1080p</t>
+          <t>64MP 2160p</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>8/12GB RAM Dimensity 6020</t>
+          <t>8GB RAM Snapdragon 888</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>5000mAh Li-Po</t>
+          <t>4500mAh Li-Ion</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Huawei</t>
+          <t>Oppo</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1753,12 +1753,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>HarmonyOS 4.0</t>
+          <t>Android 14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>6.76" 1224x2776 pixels</t>
+          <t>6.8" 1080x2520 pixels</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1768,113 +1768,113 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Kirin 9000S</t>
+          <t>12GB RAM Dimensity 9200</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>4600mAh</t>
+          <t>4300mAh Li-Po</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Huawei</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Coming soon</t>
+          <t>৳12,000.00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Not announced yet</t>
+          <t>2024, March 07</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>HarmonyOS 4.0</t>
+          <t>Android 13, One UI 5.1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>6.7" 1084x2412 pixels</t>
+          <t>6.7" 1080x2400 pixels</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>50MP 2160p</t>
+          <t>50MP 1080p</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Kirin 830</t>
+          <t>4/6GB RAM Snapdragon 680 4G</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>4600mAh</t>
+          <t>5000mAh 25W</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Energizer</t>
+          <t>OnePlus</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>৳10,000.00</t>
+          <t>Coming soon</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2024, February</t>
+          <t>Not announced yet</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Android 13</t>
+          <t>Android 14</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>6.82" 720x1640 pixels</t>
+          <t>6.78" 1240x2772 pixels</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>8MP 1080p</t>
+          <t>50MP 2160p</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2GB RAM MT6762CB</t>
+          <t>8/12GB RAM Snapdragon 8 Gen 2</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>4900mAh Li-Po</t>
+          <t>5500mAh</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Motorola</t>
+          <t>OnePlus</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>৳12,000.00</t>
+          <t>Coming soon</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2024, February 07</t>
+          <t>Not announced yet</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1884,49 +1884,49 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>6.56" 720x1612 pixels</t>
+          <t>6.82" 1440x3168 pixels</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>50MP 1080p</t>
+          <t>50MP 4320p</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>4/8GB RAM Helio G85</t>
+          <t>12-24GB RAM Snapdragon 8 Gen 3</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>6000mAh</t>
+          <t>5400mAh Li-Po</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Infinix</t>
+          <t>Vivo</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>৳12,000.00</t>
+          <t>Coming soon</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2024, February</t>
+          <t>Not announced yet</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Android 13, XOS 13</t>
+          <t>Android 14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>6.6" 720x1612 pixels</t>
+          <t>6.64" 1080x2388 pixels</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1936,19 +1936,19 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>4GB RAM Helio G36</t>
+          <t>12GB RAM Dimensity 6020</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>6000mAh</t>
+          <t>5000mAh</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>OnePlus</t>
+          <t>Realme</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1958,12 +1958,12 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2024, January 31</t>
+          <t>2024, March</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Android 13, OxygenOS 13.1</t>
+          <t>Android 14, Realme UI 5.0</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1973,44 +1973,44 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>50MP 1080p</t>
+          <t>108MP 1080p</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>4GB RAM Dimensity 6020</t>
+          <t>6/8GB RAM Dimensity 6100+</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>5000mAh Li-Po</t>
+          <t>5000mAh 45W</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Realme</t>
+          <t>Nothing</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>৳30,000.00</t>
+          <t>৳39,000.00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2024, March 02</t>
+          <t>2024, March 12</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Android 14, Realme UI 5.0</t>
+          <t>Android 14, Nothing OS 2.5</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>6.7" 1080x2400 pixels</t>
+          <t>6.7" 1080x2412 pixels</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2020,91 +2020,91 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>8GB RAM Dimensity 7050</t>
+          <t>8/12GB RAM Dimensity 7200</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>5000mAh 67W</t>
+          <t>5000mAh Li-Ion</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Realme</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>৳45,000.00 ৳42,000.00</t>
+          <t>৳20,000.00</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2024, January 29</t>
+          <t>2024, March 11</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Android 14, Realme UI 5.0</t>
+          <t>Android 14, One UI 6</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>6.7" 1080x2412 pixels</t>
+          <t>6.6" 1080x2340 pixels</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>64MP 2160p</t>
+          <t>50MP 1080p</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>8/12GB RAM Snapdragon 7s Gen 2</t>
+          <t>4/6GB RAM Dimensity 6100+</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>5000mAh Li-Po</t>
+          <t>6000mAh 25W</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Realme</t>
+          <t>Symphony</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>৳36,000.00</t>
+          <t>৳9,499.00</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2024, January 29</t>
+          <t>2024, March 03</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Android 14, Realme UI 5.0</t>
+          <t>Android 13</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>6.7" 1080x2412 pixels</t>
+          <t>6.56" 720x1600 pixels</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>50MP 2160p</t>
+          <t>52MP 1080p</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>8GB RAM Snapdragon 6 Gen 1</t>
+          <t>4GB RAM UniSOC T616</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2116,40 +2116,2560 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>Walton</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>৳17,999.00</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2024, March</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>6.82" 720 x 1640 pixels</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>50MP 1080P</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>12GB RAM Helio G85</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>5010mAh Li-po</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Meizu</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>৳95,000.00</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2024, March 02</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Android, Flyme</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>6.79" 1368x3192 pixels</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>50MP 4320p</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8 Gen 3</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>5050mAh 80W50W</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Oppo</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>৳35,000.00</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2024, March 04</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Android 14, ColorOS 14</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>8GB RAM Dimensity 7050</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>5000mAh 67W</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ZTE</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, Q1-Q2</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>6.72" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>8GB RAM Unisoc T820</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>6000mAh 33W</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ZTE</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>৳20,000.00</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, Q1-Q2</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>6.6" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>4GB RAM Unisoc SC9863A</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>5000mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>ZTE</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, Q1-Q2</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>6.72" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>108MP 2160p</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>8GB RAM Unisoc T760</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>5000mAh 33W</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>ZTE</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>৳25,000.00</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, Q1-Q2</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>6.6" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>108MP 2160p</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>8GB RAM Unisoc T760</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>5000mAh 33W</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Lava</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>৳25,000.00</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2024, March 11</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Android 13, planned upgrade to Android 14</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>6.67" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>8GB RAM Dimensity 7050</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Doogee</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2024, March</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>6.67" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>12GB RAM Dimensity 8020</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>5150mAh 120W50W</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Tecno</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2024, April 02</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Android 14, HIOS 14</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2436 pixels</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>12GB RAM Dimensity 8200</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>5000mAh 70W</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Tecno</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, May</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Android 14, HIOS 14</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>6.77" 1264x2780 pixels</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>12GB RAM Dimensity 8200</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>5000mAh 70W</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Tecno</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2024, April 02</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Android 14, HIOS 14</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2436 pixels</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Dimensity 7020</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>5000mAh 70W</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Tecno</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2024, April 02</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Android 14, HIOS 14</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2436 pixels</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Helio G99 Ultimate</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>5000mAh 70W</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>ZTE</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>৳75,000.00</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, April</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>6.9" 1188x2790 pixels</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>6GB RAM Snapdragon 7 Gen 1</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>4310mAh 33W</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>৳35,000.00</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2024, February 26</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>6.67" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>12GB RAM Snapdragon 4 Gen 2</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>5000mAh 80W</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>TCL</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, Q2</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Android 14, planned upgrade to Android 15</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>6.6" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>8GB RAM Dimensity 700</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>5010mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>TCL</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, Q2</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Android 14, planned upgrade to Android 15</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2460 pixels</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>4/6GB RAM Helio G88</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>5010mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>TCL</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, Q2</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>6.0" 540x1092 pixels</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>5MP 1080p</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>2GB RAM Helio G36</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>3000mAh 10W</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Tecno</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, March</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Android 14, HIOS 14</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2436 pixels</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>108MP 1440p</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Dimensity 6080</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>6000mAh 70W</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Energizer</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>৳30,000.00</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, October</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2460 pixels</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>60MP 2160p</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>8GB RAM Helio G99</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>28000mAh 33W</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>৳25,000.00</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2024, February 28</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Android 13, OriginOS 3</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>6.64" 1080x2388 pixels</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Dimensity 8200</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>5000mAh 120W</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>৳140,000.00</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>2024, February 22</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Android 14, HyperOS</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>6.73" 1440x3200 pixels</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>50MP 4320p</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8 Gen 3</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>5000mAh 90W80W</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>৳28,000.00</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2024, February 22</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>6.67" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>6/8GB RAM Snapdragon 4 Gen 2</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>5000mAh 44W</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Huawei</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>৳18,000.00</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2024, February 22</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>HarmonyOS 4.0</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>6.75" 720x1600 pixels</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>13MP 1080p</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Kirin 710A</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>6000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>৳55,000.00</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2024, February 22</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Android 14, HyperOS</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>12.4" 2032x3048 pixels</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>8-16GB RAM Snapdragon 8 Gen 2</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>10000mAh 120W</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>৳60,000.00</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>2024, February 22</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>6.78" 1260x2800 pixels</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>50MP 4320p</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 8 Gen 2</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>5160mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>৳40,000.00</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>2024, April 22</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>6.72" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>108MP 1080p</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>6/8GB RAM Snapdragon 685</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>5000mAh 33W</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Lava</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>6.5" 720x1600 pixels</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>8GB RAM Unisoc Tiger T616</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Oppo</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>6.82" 1440x3168 pixels</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8 Gen 3</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Oppo</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>6.82" 1440x3168 pixels</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8 Gen 2</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Oppo</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>6.78" 1264x2780 pixels</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Dimensity 9300</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>5000mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>৳12,499.00 ৳10,999.00</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>2024, February 23</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Android 14, MIUI</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>6.71" 720x1650 pixels</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>8MP 1080p</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>3-6GB RAM Helio G36</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>5000mAh 10W</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>OnePlus</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>6.72" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>108MP 1080p</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>8GB RAM Snapdragon 695 5G</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>OnePlus</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 782G</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>OnePlus</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>12GB RAM Snapdragon 695 5G</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Huawei</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>৳120,000.00</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, March</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>HarmonyOS 4.0</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>6.94" 1136x2690 pixels</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>12/16GB RAM</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>4520mAh 66W40W</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Oppo</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>12GB RAM Dimensity 8200</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>4600mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Oppo</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Dimensity 7050</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Walton</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>৳11,999.00</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>2024, February 17</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>6.8" 720 x 1612 pixels</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>52MP 1080P</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>8GB RAM UNISOC TIGER T606</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>5010mAh Li-po</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>2023, June 27</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>7.6" 1840x2208 pixels</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>48MP 2160p</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>12GB RAM Google Tensor G2</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>4821mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Oppo</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>৳30,000.00</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>2024, February 08</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Android 14, ColorOS 14</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>8GB RAM Dimensity 7050</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Energizer</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2460 pixels</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>60MP 2160p</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>28000mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>TCL</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, March</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>6.75" 720x1600 pixels</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>4GB RAM Helio G35</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>5010mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>৳55,000.00</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>2024, March 07</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>6.78" 1260x2800 pixels</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Dimensity 8200</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>5000mAh 80W</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>৳59,999.00</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>2024, March 04</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>6.78" 1260x2800 pixels</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 7 Gen 3</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>5000mAh 80W</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>8GB RAM Dimensity 7200</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>4600mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Ulefone</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>৳40,000.00</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>2024, January</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>108MP 1440p</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>12GB RAM Helio G99</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>5050mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>6.73" 1440x3200 pixels</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>50MP 4320p</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8 Gen 2</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 7s Gen 2</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>8GB RAM Snapdragon 6 Gen 1</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>6.43" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>64MP 1080p</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Dimensity 6020</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Huawei</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>HarmonyOS 4.0</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>6.76" 1224x2776 pixels</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Kirin 9000S</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>4600mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Huawei</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>HarmonyOS 4.0</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>6.7" 1084x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Kirin 830</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>4600mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Energizer</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>৳10,000.00</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>2024, February</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>6.82" 720x1640 pixels</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>8MP 1080p</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>2GB RAM MT6762CB</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>4900mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Motorola</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>৳12,000.00</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>2024, February 07</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>6.56" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>4/8GB RAM Helio G85</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>6000mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Infinix</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>৳12,000.00</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2024, February</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Android 13, XOS 13</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>6.6" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>4GB RAM Helio G36</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>6000mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>OnePlus</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>৳20,000.00</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>2024, January 31</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Android 13, OxygenOS 13.1</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>6.72" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>4GB RAM Dimensity 6020</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>৳30,000.00</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>2024, March 02</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI 5.0</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>8GB RAM Dimensity 7050</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>5000mAh 67W</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>৳45,000.00 ৳42,000.00</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>2024, January 29</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI 5.0</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 7s Gen 2</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>৳36,000.00</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>2024, January 29</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI 5.0</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>8GB RAM Snapdragon 6 Gen 1</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
           <t>Itel</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B101" t="inlineStr">
         <is>
           <t>৳12,000.00</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C101" t="inlineStr">
         <is>
           <t>2024, February</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D101" t="inlineStr">
         <is>
           <t>Android 14</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E101" t="inlineStr">
         <is>
           <t>6.6" 720x1612 pixels</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="F101" t="inlineStr">
         <is>
           <t>50MP 1080p</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="G101" t="inlineStr">
         <is>
           <t>4GB RAM Unisoc T606</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr">
+      <c r="H101" t="inlineStr">
         <is>
           <t>6000mAh Li-Po</t>
         </is>

</xml_diff>